<commit_message>
Check in the Arduino and PI
</commit_message>
<xml_diff>
--- a/Messages.xlsx
+++ b/Messages.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="NetworkTables" sheetId="1" r:id="rId1"/>
     <sheet name="FromArduinoToPi" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="PIToArduino" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">NetworkTables!$A$1:$K$60</definedName>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="69">
   <si>
     <t>blob0</t>
   </si>
@@ -209,6 +209,33 @@
   </si>
   <si>
     <t>fromPi</t>
+  </si>
+  <si>
+    <t>toPi</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>sensorLevel</t>
+  </si>
+  <si>
+    <t>prox01</t>
+  </si>
+  <si>
+    <t>prox02</t>
+  </si>
+  <si>
+    <t>prox03</t>
+  </si>
+  <si>
+    <t>prox04</t>
+  </si>
+  <si>
+    <t>prox05</t>
+  </si>
+  <si>
+    <t>prox06</t>
   </si>
 </sst>
 </file>
@@ -560,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B496C069-0F1B-49D1-A5C7-6A491255A782}">
-  <dimension ref="B2:G60"/>
+  <dimension ref="B2:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,6 +1326,80 @@
       </c>
       <c r="D60" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>60</v>
+      </c>
+      <c r="C62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>60</v>
+      </c>
+      <c r="C63" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>60</v>
+      </c>
+      <c r="C64" t="s">
+        <v>64</v>
+      </c>
+      <c r="D64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>60</v>
+      </c>
+      <c r="C65" t="s">
+        <v>65</v>
+      </c>
+      <c r="D65" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>60</v>
+      </c>
+      <c r="C66" t="s">
+        <v>66</v>
+      </c>
+      <c r="D66" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>60</v>
+      </c>
+      <c r="C67" t="s">
+        <v>67</v>
+      </c>
+      <c r="D67" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>60</v>
+      </c>
+      <c r="C68" t="s">
+        <v>68</v>
+      </c>
+      <c r="D68" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1311,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD70F17D-1660-42D7-BF0E-30B5259A26A3}">
   <dimension ref="C2:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:I18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,7 +1471,7 @@
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6">
-        <f t="shared" ref="C6:C33" si="0">C5+1</f>
+        <f t="shared" ref="C6:C18" si="0">C5+1</f>
         <v>4</v>
       </c>
       <c r="D6" t="s">
@@ -1498,7 +1599,7 @@
   <dimension ref="C2:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="C3" sqref="C3:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,7 +1663,7 @@
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6">
-        <f t="shared" ref="C6:C18" si="0">C5+1</f>
+        <f t="shared" ref="C6:C9" si="0">C5+1</f>
         <v>4</v>
       </c>
       <c r="D6" t="s">

</xml_diff>